<commit_message>
Update bedrock-translate with new samples and results
</commit_message>
<xml_diff>
--- a/bedrock-translate/final_results/translation_document_sample2_20250806_130701.xlsx
+++ b/bedrock-translate/final_results/translation_document_sample2_20250806_130701.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joohyery/Documents/Dev/amazon-bedrock-samples-joohyery/bedrock-translate/final_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00A3BE4-7CE7-C044-8095-5E0820FC1C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0548B362-8A1F-4E48-A0E9-068040DE8B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="4500" windowWidth="34920" windowHeight="27200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27420" yWindow="500" windowWidth="34920" windowHeight="27140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Translation" sheetId="1" r:id="rId1"/>
@@ -742,7 +742,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -891,7 +891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="137" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -912,7 +912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="127" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>

</xml_diff>